<commit_message>
plotted dyhrman 2012 go in nb
</commit_message>
<xml_diff>
--- a/data/thaps-ref/dyherman-thaps-cc-go.xlsx
+++ b/data/thaps-ref/dyherman-thaps-cc-go.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="dyherman-thaps-cc-go" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="507">
   <si>
     <t xml:space="preserve">Peptides</t>
   </si>
@@ -1512,7 +1512,16 @@
     <t xml:space="preserve">GO term</t>
   </si>
   <si>
+    <t xml:space="preserve">Unused</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chloroplast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">obsolete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">both nucleus and cytoplasm</t>
   </si>
   <si>
     <t xml:space="preserve">Membrane</t>
@@ -1548,6 +1557,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1635,11 +1645,11 @@
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="74.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="74.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4375,13 +4385,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H95"/>
+  <dimension ref="A1:I80"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.66"/>
@@ -4405,6 +4415,9 @@
       <c r="D1" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>496</v>
+      </c>
       <c r="F1" s="0" t="s">
         <v>0</v>
       </c>
@@ -4417,7 +4430,23 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>496</v>
+        <v>497</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <f aca="false">SUM(B3:B14)</f>
+        <v>696</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>498</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4430,6 +4459,18 @@
       <c r="D3" s="0" t="s">
         <v>220</v>
       </c>
+      <c r="F3" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>499</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="n">
@@ -4441,6 +4482,15 @@
       <c r="D4" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="F4" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="n">
@@ -4452,6 +4502,15 @@
       <c r="D5" s="0" t="s">
         <v>38</v>
       </c>
+      <c r="F5" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="n">
@@ -4463,6 +4522,15 @@
       <c r="D6" s="0" t="s">
         <v>40</v>
       </c>
+      <c r="F6" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="n">
@@ -4474,6 +4542,15 @@
       <c r="D7" s="0" t="s">
         <v>66</v>
       </c>
+      <c r="F7" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="n">
@@ -4485,6 +4562,15 @@
       <c r="D8" s="0" t="s">
         <v>76</v>
       </c>
+      <c r="F8" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="n">
@@ -4496,6 +4582,15 @@
       <c r="D9" s="0" t="s">
         <v>114</v>
       </c>
+      <c r="F9" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="n">
@@ -4507,6 +4602,15 @@
       <c r="D10" s="0" t="s">
         <v>116</v>
       </c>
+      <c r="F10" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="n">
@@ -4518,6 +4622,15 @@
       <c r="D11" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="F11" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="n">
@@ -4529,6 +4642,15 @@
       <c r="D12" s="0" t="s">
         <v>148</v>
       </c>
+      <c r="F12" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="n">
@@ -4540,6 +4662,15 @@
       <c r="D13" s="0" t="s">
         <v>178</v>
       </c>
+      <c r="F13" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="n">
@@ -4551,10 +4682,32 @@
       <c r="D14" s="0" t="s">
         <v>170</v>
       </c>
+      <c r="F14" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>497</v>
+        <v>500</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <f aca="false">SUM(B16:B28)</f>
+        <v>1081</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4567,6 +4720,15 @@
       <c r="D16" s="0" t="s">
         <v>58</v>
       </c>
+      <c r="F16" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="n">
@@ -4578,6 +4740,15 @@
       <c r="D17" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="F17" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="n">
@@ -4590,13 +4761,13 @@
         <v>18</v>
       </c>
       <c r="F18" s="0" t="n">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>35</v>
+        <v>101</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>36</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4609,6 +4780,15 @@
       <c r="D19" s="0" t="s">
         <v>32</v>
       </c>
+      <c r="F19" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="n">
@@ -4620,6 +4800,15 @@
       <c r="D20" s="0" t="s">
         <v>30</v>
       </c>
+      <c r="F20" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="n">
@@ -4631,6 +4820,15 @@
       <c r="D21" s="0" t="s">
         <v>138</v>
       </c>
+      <c r="F21" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="n">
@@ -4643,13 +4841,13 @@
         <v>160</v>
       </c>
       <c r="F22" s="0" t="n">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>43</v>
+        <v>139</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>44</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4662,6 +4860,15 @@
       <c r="D23" s="0" t="s">
         <v>200</v>
       </c>
+      <c r="F23" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="n">
@@ -4674,13 +4881,13 @@
         <v>78</v>
       </c>
       <c r="F24" s="0" t="n">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>47</v>
+        <v>151</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>48</v>
+        <v>152</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4694,13 +4901,13 @@
         <v>88</v>
       </c>
       <c r="F25" s="0" t="n">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>49</v>
+        <v>157</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>50</v>
+        <v>158</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4714,13 +4921,13 @@
         <v>96</v>
       </c>
       <c r="F26" s="0" t="n">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>51</v>
+        <v>161</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>52</v>
+        <v>162</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4733,196 +4940,274 @@
       <c r="D27" s="0" t="s">
         <v>110</v>
       </c>
+      <c r="F27" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="F28" s="0" t="n">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>55</v>
+        <v>165</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>56</v>
+        <v>166</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>498</v>
+        <v>501</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <f aca="false">SUM(B30:B50)</f>
+        <v>535</v>
       </c>
       <c r="F29" s="0" t="n">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>69</v>
+        <v>167</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>70</v>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="n">
-        <v>25</v>
+        <v>182</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>61</v>
+        <v>15</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>62</v>
+        <v>16</v>
       </c>
       <c r="F31" s="0" t="n">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>73</v>
+        <v>195</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>74</v>
+        <v>196</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="n">
-        <v>182</v>
+        <v>34</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>16</v>
+        <v>42</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G32" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="H32" s="0" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="n">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>42</v>
+        <v>54</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G33" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="H33" s="0" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C34" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>54</v>
-      </c>
       <c r="F34" s="0" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>79</v>
+        <v>189</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>80</v>
+        <v>190</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="n">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>28</v>
+        <v>46</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G35" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="H35" s="0" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="n">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>45</v>
+        <v>97</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>46</v>
+        <v>98</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G36" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="H36" s="0" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>98</v>
+        <v>104</v>
+      </c>
+      <c r="F37" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="H37" s="0" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>104</v>
+        <v>84</v>
+      </c>
+      <c r="F38" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G38" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="H38" s="0" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="n">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>83</v>
+        <v>217</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>84</v>
+        <v>218</v>
       </c>
       <c r="F39" s="0" t="n">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>89</v>
+        <v>207</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>90</v>
+        <v>208</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>217</v>
+        <v>121</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>218</v>
-      </c>
-      <c r="F40" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="G40" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="H40" s="0" t="s">
-        <v>92</v>
+        <v>122</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="0" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4930,10 +5215,10 @@
         <v>11</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4941,10 +5226,10 @@
         <v>11</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4952,19 +5237,10 @@
         <v>11</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="F44" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="G44" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="H44" s="0" t="s">
-        <v>100</v>
+        <v>128</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4972,634 +5248,391 @@
         <v>11</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="F45" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="G45" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="H45" s="0" t="s">
-        <v>102</v>
+        <v>136</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>135</v>
+        <v>181</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>136</v>
+        <v>182</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F47" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="G47" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="H47" s="0" t="s">
-        <v>106</v>
+      <c r="B47" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
-        <v>499</v>
-      </c>
-      <c r="F48" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="G48" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="H48" s="0" t="s">
-        <v>108</v>
+      <c r="B48" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="0" t="n">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>67</v>
+        <v>145</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>68</v>
+        <v>146</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="n">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>71</v>
+        <v>211</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="F50" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="G50" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="H50" s="0" t="s">
-        <v>112</v>
+        <v>212</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>502</v>
+      </c>
       <c r="B51" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="C51" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="D51" s="0" t="s">
-        <v>82</v>
+        <f aca="false">SUM(B52:B55)</f>
+        <v>74</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="C52" s="0" t="s">
+      <c r="C55" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="D52" s="0" t="s">
+      <c r="D55" s="0" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F53" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="G53" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="H53" s="0" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
-        <v>500</v>
-      </c>
-    </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>503</v>
+      </c>
       <c r="B56" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="C56" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="D56" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="F56" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="G56" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="H56" s="0" t="s">
-        <v>124</v>
+        <f aca="false">SUM(B57:B61)</f>
+        <v>69</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="C57" s="0" t="s">
+      <c r="C58" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="D57" s="0" t="s">
+      <c r="D58" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="F57" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="G57" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="H57" s="0" t="s">
-        <v>140</v>
-      </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
-        <v>501</v>
-      </c>
-      <c r="F59" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="G59" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="H59" s="0" t="s">
-        <v>144</v>
+      <c r="B59" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="0" t="n">
-        <v>170</v>
+        <v>4</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>19</v>
+        <v>201</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="F60" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="G60" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="H60" s="0" t="s">
-        <v>146</v>
+        <v>202</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="0" t="n">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>33</v>
+        <v>89</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>504</v>
+      </c>
       <c r="B62" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="C62" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="D62" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="F62" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="G62" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="H62" s="0" t="s">
-        <v>150</v>
+        <f aca="false">SUM(B63:B65)</f>
+        <v>247</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
-        <v>502</v>
-      </c>
-      <c r="F63" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="G63" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="H63" s="0" t="s">
-        <v>152</v>
+      <c r="B63" s="0" t="n">
+        <v>170</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="0" t="n">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>141</v>
+        <v>33</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="F64" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="G64" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="H64" s="0" t="s">
-        <v>154</v>
+        <v>34</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="0" t="n">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>155</v>
+        <v>63</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>156</v>
+        <v>64</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>505</v>
+      </c>
       <c r="B66" s="0" t="n">
-        <v>238</v>
-      </c>
-      <c r="C66" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D66" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F66" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="G66" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="H66" s="0" t="s">
-        <v>158</v>
+        <f aca="false">SUM(B67:B73)</f>
+        <v>290</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="0" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>93</v>
+        <v>141</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>94</v>
+        <v>142</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="0" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>172</v>
-      </c>
-      <c r="F68" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="G68" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="H68" s="0" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="0" t="n">
-        <v>7</v>
+        <v>238</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>173</v>
+        <v>11</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="F69" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="G69" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="H69" s="0" t="s">
-        <v>164</v>
+        <v>12</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="0" t="n">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>213</v>
+        <v>93</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>214</v>
-      </c>
-      <c r="F70" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="G70" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="H70" s="0" t="s">
-        <v>166</v>
+        <v>94</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F71" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="G71" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="H71" s="0" t="s">
-        <v>168</v>
+      <c r="B71" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="D71" s="0" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
-        <v>503</v>
+      <c r="B72" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="D72" s="0" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="0" t="n">
-        <v>697</v>
+        <v>4</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>3</v>
+        <v>213</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>4</v>
+        <v>214</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>506</v>
+      </c>
       <c r="B74" s="0" t="n">
-        <v>494</v>
-      </c>
-      <c r="C74" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D74" s="0" t="s">
-        <v>8</v>
+        <f aca="false">SUM(B75:B80)</f>
+        <v>1457</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="0" t="n">
-        <v>149</v>
+        <v>697</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="0" t="n">
-        <v>100</v>
+        <v>494</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="0" t="n">
-        <v>93</v>
+        <v>149</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="F77" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="G77" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="H77" s="0" t="s">
-        <v>180</v>
+        <v>22</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="0" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>187</v>
+        <v>23</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="F78" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="G78" s="0" t="s">
-        <v>181</v>
-      </c>
-      <c r="H78" s="0" t="s">
-        <v>182</v>
+        <v>24</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C79" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="D79" s="0" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B80" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C79" s="0" t="s">
+      <c r="C80" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="D79" s="0" t="s">
+      <c r="D80" s="0" t="s">
         <v>120</v>
-      </c>
-      <c r="F79" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="G79" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="H79" s="0" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F80" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="G80" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="H80" s="0" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F82" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="G82" s="0" t="s">
-        <v>189</v>
-      </c>
-      <c r="H82" s="0" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F83" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="G83" s="0" t="s">
-        <v>191</v>
-      </c>
-      <c r="H83" s="0" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F84" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="G84" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="H84" s="0" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F85" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="G85" s="0" t="s">
-        <v>195</v>
-      </c>
-      <c r="H85" s="0" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F86" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="G86" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="H86" s="0" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F88" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="G88" s="0" t="s">
-        <v>201</v>
-      </c>
-      <c r="H88" s="0" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F89" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="G89" s="0" t="s">
-        <v>203</v>
-      </c>
-      <c r="H89" s="0" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F90" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="G90" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="H90" s="0" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F91" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="G91" s="0" t="s">
-        <v>207</v>
-      </c>
-      <c r="H91" s="0" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F92" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="G92" s="0" t="s">
-        <v>209</v>
-      </c>
-      <c r="H92" s="0" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F93" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="G93" s="0" t="s">
-        <v>211</v>
-      </c>
-      <c r="H93" s="0" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F95" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="G95" s="0" t="s">
-        <v>215</v>
-      </c>
-      <c r="H95" s="0" t="s">
-        <v>216</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -5612,17 +5645,90 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>497</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>500</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>501</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>502</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>503</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>504</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>505</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>506</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>1457</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
didnt change the ptm fig
</commit_message>
<xml_diff>
--- a/data/thaps-ref/dyherman-thaps-cc-go.xlsx
+++ b/data/thaps-ref/dyherman-thaps-cc-go.xlsx
@@ -1645,7 +1645,7 @@
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.71"/>
@@ -4372,7 +4372,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -4391,7 +4391,7 @@
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.66"/>
@@ -5632,7 +5632,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -5648,10 +5648,10 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -5728,7 +5728,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>